<commit_message>
fix slow typing and add fallback mechanic
</commit_message>
<xml_diff>
--- a/data/SendColdEmailTest3.xlsx
+++ b/data/SendColdEmailTest3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vietlh/Desktop/Workshop/auto/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vietlh/Desktop/Workshop/auto/UIMailSender/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Company Name</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>vietluonghoang@gmail.com</t>
+  </si>
+  <si>
+    <t>Hoang Dup</t>
   </si>
 </sst>
 </file>
@@ -444,10 +447,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -529,47 +532,57 @@
     </row>
     <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="2" t="s">
-        <v>20</v>
+      <c r="E4" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="1" t="s">
-        <v>24</v>
+      <c r="E5" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1" t="s">
         <v>28</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E4" r:id="rId1"/>
+    <hyperlink ref="E5" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>